<commit_message>
Adding Registartion Page Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dsalgo.xlsx
+++ b/src/test/resources/testdata/dsalgo.xlsx
@@ -5,19 +5,20 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="+2TIMFMYTdo1Hbl/3NBbMlXxZHFsxiZxpRhXEo9ugJs="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="S5eSbksyh+Ead8Ij/m+gfrTe35+Kl8os24mTlGTvbAU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>input</t>
   </si>
@@ -51,12 +52,54 @@
   <si>
     <t>t</t>
   </si>
+  <si>
+    <t>Username:</t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>Password confirmation:</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>ninja tester</t>
+  </si>
+  <si>
+    <t>ninja@123</t>
+  </si>
+  <si>
+    <t>ninjatesterss</t>
+  </si>
+  <si>
+    <t>nin@1</t>
+  </si>
+  <si>
+    <t>ninja@12345</t>
+  </si>
+  <si>
+    <t>ninjatestersssss</t>
+  </si>
+  <si>
+    <t>numpyninjatester1</t>
+  </si>
+  <si>
+    <t>numpyninjatester2</t>
+  </si>
+  <si>
+    <t>numpyninjatester3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -80,6 +123,11 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -104,6 +152,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -118,6 +169,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2371,4 +2426,148 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="35.86"/>
+    <col customWidth="1" min="3" max="3" width="18.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.23456789E9</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.23456789E9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding all the 68 test cases of Tree Module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dsalgo.xlsx
+++ b/src/test/resources/testdata/dsalgo.xlsx
@@ -6,19 +6,20 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Sheet4" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="S5eSbksyh+Ead8Ij/m+gfrTe35+Kl8os24mTlGTvbAU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="eO6TJTwmAUp//DgLAlLctmmrxxNLhf25iWd6/KAzJbk="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>input</t>
   </si>
@@ -51,6 +52,21 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>Pyhton Code:</t>
+  </si>
+  <si>
+    <t>Valid Python Code</t>
+  </si>
+  <si>
+    <t>print("This is a valid python code")</t>
+  </si>
+  <si>
+    <t>Incali Python Code</t>
+  </si>
+  <si>
+    <t>p("Invalid Code")</t>
   </si>
   <si>
     <t>Username:</t>
@@ -173,6 +189,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1432,6 +1452,27 @@
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2444,6 +2485,150 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.23456789E9</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.23456789E9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.43"/>
+    <col customWidth="1" min="2" max="2" width="35.86"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2451,120 +2636,16 @@
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1.23456789E9</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1.23456789E9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Array Practice Questions updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/dsalgo.xlsx
+++ b/src/test/resources/testdata/dsalgo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7005"/>
+    <workbookView windowWidth="20490" windowHeight="7005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>input</t>
   </si>
@@ -126,6 +126,62 @@
   </si>
   <si>
     <t>numpyninjatester3</t>
+  </si>
+  <si>
+    <t>Search the array</t>
+  </si>
+  <si>
+    <t>lst=[ 1, 6, 3, 5, 3, 4 ] 
+#checking if element 7 is present
+# in the given list or not
+i=7 
+# if element present then return
+# exist otherwise not exist
+if i in lst: 
+    print("exist") 
+else: 
+    print("not exist")</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>def search(input_list, num): 
+    if (num in input_list):
+        print("Element Found")
+    else:
+        print("Not Found")
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>Find Numbers with Even Number of Digits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])   </t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+squares_list = []
+for i in range(0, len(nums)):
+square = nums[i] * nums[i];
+squares_list.append(square)
+\b
+\b
+sorted_squares_list = sorted(squares_list)
+print sorted_squares_list;
+return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
   </si>
 </sst>
 </file>
@@ -138,13 +194,19 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.25"/>
+      <color rgb="FF000000"/>
+      <name val="docs-Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="8"/>
@@ -629,144 +691,150 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1243,7 +1311,7 @@
   <sheetPr/>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1253,26 +1321,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="1" spans="1:2">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="7" customFormat="1" spans="1:2">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="1" spans="1:2">
-      <c r="A3" s="5" t="s">
+    <row r="3" s="7" customFormat="1" spans="1:2">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2280,26 +2348,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3369,7 +3437,7 @@
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B5" t="s">
@@ -3478,15 +3546,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="23.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="36.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="35.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3511,6 +3579,38 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" ht="142" customHeight="1" spans="1:2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" ht="102" customHeight="1" spans="1:2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" ht="151" customHeight="1" spans="1:2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" ht="129" customHeight="1" spans="1:2">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>